<commit_message>
adding chapter 12 notes
</commit_message>
<xml_diff>
--- a/NanoDegreeProgress.xlsx
+++ b/NanoDegreeProgress.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="248">
   <si>
     <t>Programming Fundamentals and the Web</t>
   </si>
@@ -2072,9 +2072,6 @@
   </si>
   <si>
     <t>Build a Portfolio Site</t>
-  </si>
-  <si>
-    <t>60-17</t>
   </si>
 </sst>
 </file>
@@ -2959,8 +2956,8 @@
   <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3149,8 +3146,9 @@
       <c r="G10" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="H10" t="s">
-        <v>248</v>
+      <c r="H10">
+        <f>60-17</f>
+        <v>43</v>
       </c>
       <c r="L10" s="35"/>
     </row>
@@ -3170,6 +3168,10 @@
       <c r="G11" s="37" t="s">
         <v>21</v>
       </c>
+      <c r="H11">
+        <f>60-23</f>
+        <v>37</v>
+      </c>
       <c r="L11" s="35"/>
     </row>
     <row r="12" spans="1:12">
@@ -3187,6 +3189,9 @@
       </c>
       <c r="G12" s="37" t="s">
         <v>21</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
       </c>
       <c r="L12" s="35"/>
     </row>

</xml_diff>